<commit_message>
Implement configuration management and enhance authentication features. Added Google Sheets integration for attendance exports, improved session handling, and introduced email notification system. Refactored app.py for better organization and maintainability.
</commit_message>
<xml_diff>
--- a/excel_exports/DSAJ_ENTC_B.TechB.xlsx
+++ b/excel_exports/DSAJ_ENTC_B.TechB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,6 +549,41 @@
           <t>Attendance %</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_x</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_y</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_x.1</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_y.1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_x.2</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_y.2</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -655,10 +690,45 @@
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W2" t="n">
         <v>0</v>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -766,10 +836,45 @@
         <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W3" t="n">
         <v>0</v>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -877,10 +982,45 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -988,10 +1128,45 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W5" t="n">
         <v>0</v>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -1099,10 +1274,45 @@
         <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W6" t="n">
         <v>0</v>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -1210,10 +1420,45 @@
         <v>3</v>
       </c>
       <c r="V7" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W7" t="n">
-        <v>17.6</v>
+        <v>13.6</v>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -1321,10 +1566,193 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W8" t="n">
         <v>0</v>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>EC4226</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Abhishek Pathak</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>abhipathak2513@gmail.com</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>4</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>EC4237</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Shubham Pitekar</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>shubhampitekar2323@gmail.com</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>4</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Face Recognition Accuracy Optimization Guide and enhance attendance features
- Introduced a comprehensive guide for optimizing face recognition accuracy, including model selection, threshold tuning, and camera setup recommendations.
- Updated the attendance feature to allow manual verification of recognized students before marking attendance, improving user experience and accuracy.
- Enhanced the face detection functionality to support multiple detector backends, providing flexibility in accuracy and performance.
- Improved UI elements for better user guidance on recognition settings and accuracy tips.
</commit_message>
<xml_diff>
--- a/excel_exports/DSAJ_ENTC_B.TechB.xlsx
+++ b/excel_exports/DSAJ_ENTC_B.TechB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AH10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,55 +531,75 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
+          <t>2025-11-21_x.1</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Attendance %</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_x</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_y</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_x.1</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_y.1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_x.2</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_y.2</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_x.3</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-22_y.3</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>2025-11-21_y.1</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Attendance %</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>2025-11-22_x</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>2025-11-22_y</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>2025-11-22_x.1</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>2025-11-22_y.1</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>2025-11-22_x.2</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>2025-11-22_y.2</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>2025-11-22</t>
         </is>
@@ -687,13 +707,13 @@
         </is>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V2" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="W2" t="n">
-        <v>0</v>
+        <v>7.4</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
@@ -726,6 +746,26 @@
         </is>
       </c>
       <c r="AD2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
         <is>
           <t>❌</t>
         </is>
@@ -836,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="W3" t="n">
         <v>0</v>
@@ -872,6 +912,26 @@
         </is>
       </c>
       <c r="AD3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
         <is>
           <t>❌</t>
         </is>
@@ -982,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
@@ -1018,6 +1078,26 @@
         </is>
       </c>
       <c r="AD4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
         <is>
           <t>❌</t>
         </is>
@@ -1128,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="W5" t="n">
         <v>0</v>
@@ -1164,6 +1244,26 @@
         </is>
       </c>
       <c r="AD5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
         <is>
           <t>❌</t>
         </is>
@@ -1271,13 +1371,13 @@
         </is>
       </c>
       <c r="U6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V6" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="W6" t="n">
-        <v>0</v>
+        <v>7.4</v>
       </c>
       <c r="X6" t="inlineStr">
         <is>
@@ -1310,6 +1410,26 @@
         </is>
       </c>
       <c r="AD6" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
         <is>
           <t>❌</t>
         </is>
@@ -1417,13 +1537,13 @@
         </is>
       </c>
       <c r="U7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V7" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="W7" t="n">
-        <v>13.6</v>
+        <v>18.5</v>
       </c>
       <c r="X7" t="inlineStr">
         <is>
@@ -1456,6 +1576,26 @@
         </is>
       </c>
       <c r="AD7" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
         <is>
           <t>❌</t>
         </is>
@@ -1566,7 +1706,7 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="W8" t="n">
         <v>0</v>
@@ -1602,6 +1742,26 @@
         </is>
       </c>
       <c r="AD8" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
         <is>
           <t>❌</t>
         </is>
@@ -1644,7 +1804,7 @@
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="W9" t="n">
         <v>0</v>
@@ -1676,6 +1836,26 @@
         </is>
       </c>
       <c r="AD9" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
         <is>
           <t>❌</t>
         </is>
@@ -1715,13 +1895,13 @@
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V10" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="W10" t="n">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr">
@@ -1750,6 +1930,26 @@
         </is>
       </c>
       <c r="AD10" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>⏸️</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="AH10" t="inlineStr">
         <is>
           <t>❌</t>
         </is>

</xml_diff>